<commit_message>
fix and update All
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/template/TransactionExport.xlsx
+++ b/src/main/webapp/WEB-INF/template/TransactionExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\cms\cms_freelancer\src\main\webapp\WEB-INF\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8EDF37-E741-42FD-94B1-2E2FC926D7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4F4359-B806-4D44-BE4D-280823CAA6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>USER</author>
     <author>DucLN</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{348AB693-2C4E-49AD-AB0B-B454E1B3ED16}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5C1B39B4-4F27-47C4-BDDB-D4CA16D7903D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="I2")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="1" shapeId="0" xr:uid="{348AB693-2C4E-49AD-AB0B-B454E1B3ED16}">
       <text>
         <r>
           <rPr>
@@ -50,11 +75,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="I2")</t>
+jx:area(lastCell="I5")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{C287C509-C5B3-411D-9C06-BBB6D16D2EC6}">
+    <comment ref="A5" authorId="1" shapeId="0" xr:uid="{C287C509-C5B3-411D-9C06-BBB6D16D2EC6}">
       <text>
         <r>
           <rPr>
@@ -74,7 +99,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="item.transactionExcel" var="t" lastCell="I2")</t>
+jx:each(items="item.transactionExcel" var="t" lastCell="I5")</t>
         </r>
       </text>
     </comment>
@@ -83,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>${t.stt}</t>
   </si>
@@ -115,45 +140,47 @@
     <t>Số tiền chiết khấu</t>
   </si>
   <si>
+    <t>${t.discountMoney}</t>
+  </si>
+  <si>
+    <t>Số tiền giao dịch</t>
+  </si>
+  <si>
+    <t>${t.finalMoney}</t>
+  </si>
+  <si>
+    <t>Thời gian giao dịch</t>
+  </si>
+  <si>
+    <t>${t.transactionTimeString}</t>
+  </si>
+  <si>
+    <t>${t.paymentTypeName}</t>
+  </si>
+  <si>
+    <t>QUẢN LÝ THÔNG TIN GIAO DỊCH</t>
+  </si>
+  <si>
+    <t>Phương thức thanh toán</t>
+  </si>
+  <si>
     <t>${t.amountOfMoney}</t>
-  </si>
-  <si>
-    <t>${t.discountMoney}</t>
-  </si>
-  <si>
-    <t>Số tiền giao dịch</t>
-  </si>
-  <si>
-    <t>${t.finalMoney}</t>
-  </si>
-  <si>
-    <t>Loại giao dịch</t>
-  </si>
-  <si>
-    <t>Thời gian giao dịch</t>
-  </si>
-  <si>
-    <t>${t.transactionTimeString}</t>
-  </si>
-  <si>
-    <t>${t.paymentTypeName}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;đ&quot;"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="9"/>
@@ -168,16 +195,54 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,18 +250,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,73 +579,101 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>